<commit_message>
start doc at line 3 instead of 11
</commit_message>
<xml_diff>
--- a/assets/templates/import-rights-template.xlsx
+++ b/assets/templates/import-rights-template.xlsx
@@ -574,13 +574,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A9:AH80"/>
+  <dimension ref="A1:AH72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>
@@ -602,140 +602,388 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="L1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+    </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="L9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="U10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="V10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="W10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="X10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD10" s="8"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="8"/>
-      <c r="AH10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="12"/>
       <c r="K11" s="13"/>
       <c r="L11" s="11"/>
@@ -766,9 +1014,9 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -788,24 +1036,24 @@
       <c r="AB12" s="11"/>
       <c r="AC12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
       <c r="J13" s="12"/>
       <c r="K13" s="13"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
@@ -819,24 +1067,24 @@
       <c r="AB13" s="11"/>
       <c r="AC13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="11"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="12"/>
       <c r="K14" s="13"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
@@ -853,137 +1101,137 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="12"/>
       <c r="K15" s="13"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="12"/>
       <c r="K16" s="13"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="12"/>
       <c r="K17" s="13"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
       <c r="K18" s="13"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="11"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
       <c r="J19" s="12"/>
       <c r="K19" s="13"/>
       <c r="L19" s="11"/>
@@ -992,31 +1240,31 @@
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
-      <c r="AC19" s="11"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
       <c r="J20" s="12"/>
-      <c r="K20" s="15"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
@@ -1041,19 +1289,19 @@
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
       <c r="J21" s="12"/>
       <c r="K21" s="13"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
       <c r="T21" s="11"/>
@@ -1070,21 +1318,21 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="16"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
       <c r="J22" s="12"/>
       <c r="K22" s="13"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
@@ -1113,25 +1361,25 @@
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
       <c r="U23" s="17"/>
       <c r="V23" s="17"/>
       <c r="W23" s="17"/>
-      <c r="X23" s="17"/>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="17"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
       <c r="AA23" s="17"/>
       <c r="AB23" s="17"/>
       <c r="AC23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -1144,25 +1392,25 @@
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
       <c r="U24" s="17"/>
       <c r="V24" s="17"/>
       <c r="W24" s="17"/>
-      <c r="X24" s="17"/>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="17"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
       <c r="AA24" s="17"/>
       <c r="AB24" s="17"/>
       <c r="AC24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
@@ -1175,25 +1423,25 @@
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="17"/>
-      <c r="V25" s="17"/>
-      <c r="W25" s="17"/>
-      <c r="X25" s="17"/>
-      <c r="Y25" s="17"/>
-      <c r="Z25" s="17"/>
-      <c r="AA25" s="17"/>
-      <c r="AB25" s="17"/>
-      <c r="AC25" s="17"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
@@ -1206,21 +1454,21 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-      <c r="U26" s="17"/>
-      <c r="V26" s="17"/>
-      <c r="W26" s="17"/>
-      <c r="X26" s="17"/>
-      <c r="Y26" s="17"/>
-      <c r="Z26" s="17"/>
-      <c r="AA26" s="17"/>
-      <c r="AB26" s="17"/>
-      <c r="AC26" s="17"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
@@ -1233,7 +1481,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="12"/>
-      <c r="K27" s="13"/>
+      <c r="K27" s="15"/>
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
@@ -1264,25 +1512,25 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="12"/>
-      <c r="K28" s="13"/>
+      <c r="K28" s="15"/>
       <c r="L28" s="11"/>
       <c r="M28" s="11"/>
       <c r="N28" s="11"/>
       <c r="O28" s="11"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="11"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9"/>
@@ -1295,25 +1543,25 @@
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="12"/>
-      <c r="K29" s="13"/>
+      <c r="K29" s="15"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11"/>
       <c r="P29" s="11"/>
       <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="11"/>
-      <c r="AA29" s="11"/>
-      <c r="AB29" s="11"/>
-      <c r="AC29" s="11"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9"/>
@@ -1326,25 +1574,25 @@
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="12"/>
-      <c r="K30" s="13"/>
+      <c r="K30" s="15"/>
       <c r="L30" s="11"/>
       <c r="M30" s="11"/>
       <c r="N30" s="11"/>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="11"/>
-      <c r="AB30" s="11"/>
-      <c r="AC30" s="11"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="17"/>
+      <c r="AA30" s="17"/>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9"/>
@@ -1357,29 +1605,29 @@
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="12"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="15"/>
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
       <c r="U31" s="17"/>
       <c r="V31" s="17"/>
       <c r="W31" s="17"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="11"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
       <c r="AA31" s="17"/>
       <c r="AB31" s="17"/>
       <c r="AC31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
-      <c r="B32" s="18"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
@@ -1388,29 +1636,29 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
       <c r="J32" s="12"/>
-      <c r="K32" s="13"/>
+      <c r="K32" s="15"/>
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
       <c r="N32" s="11"/>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
       <c r="U32" s="17"/>
       <c r="V32" s="17"/>
       <c r="W32" s="17"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
       <c r="AA32" s="17"/>
       <c r="AB32" s="17"/>
       <c r="AC32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9"/>
-      <c r="B33" s="18"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
@@ -1426,12 +1674,12 @@
       <c r="O33" s="11"/>
       <c r="P33" s="11"/>
       <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
       <c r="X33" s="11"/>
       <c r="Y33" s="11"/>
       <c r="Z33" s="11"/>
@@ -1441,7 +1689,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9"/>
-      <c r="B34" s="18"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
@@ -1481,25 +1729,25 @@
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="12"/>
-      <c r="K35" s="15"/>
+      <c r="K35" s="13"/>
       <c r="L35" s="11"/>
       <c r="M35" s="11"/>
       <c r="N35" s="11"/>
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
       <c r="Q35" s="11"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="17"/>
-      <c r="V35" s="17"/>
-      <c r="W35" s="17"/>
-      <c r="X35" s="17"/>
-      <c r="Y35" s="17"/>
-      <c r="Z35" s="17"/>
-      <c r="AA35" s="17"/>
-      <c r="AB35" s="17"/>
-      <c r="AC35" s="17"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9"/>
@@ -1512,25 +1760,25 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="12"/>
-      <c r="K36" s="15"/>
+      <c r="K36" s="13"/>
       <c r="L36" s="11"/>
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
       <c r="Q36" s="11"/>
-      <c r="R36" s="17"/>
-      <c r="S36" s="17"/>
-      <c r="T36" s="17"/>
-      <c r="U36" s="17"/>
-      <c r="V36" s="17"/>
-      <c r="W36" s="17"/>
-      <c r="X36" s="17"/>
-      <c r="Y36" s="17"/>
-      <c r="Z36" s="17"/>
-      <c r="AA36" s="17"/>
-      <c r="AB36" s="17"/>
-      <c r="AC36" s="17"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9"/>
@@ -1543,7 +1791,7 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="12"/>
-      <c r="K37" s="15"/>
+      <c r="K37" s="13"/>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
       <c r="N37" s="11"/>
@@ -1556,12 +1804,12 @@
       <c r="U37" s="17"/>
       <c r="V37" s="17"/>
       <c r="W37" s="17"/>
-      <c r="X37" s="17"/>
-      <c r="Y37" s="17"/>
-      <c r="Z37" s="17"/>
-      <c r="AA37" s="17"/>
-      <c r="AB37" s="17"/>
-      <c r="AC37" s="17"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9"/>
@@ -1574,7 +1822,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
       <c r="J38" s="12"/>
-      <c r="K38" s="15"/>
+      <c r="K38" s="13"/>
       <c r="L38" s="11"/>
       <c r="M38" s="11"/>
       <c r="N38" s="11"/>
@@ -1587,12 +1835,12 @@
       <c r="U38" s="17"/>
       <c r="V38" s="17"/>
       <c r="W38" s="17"/>
-      <c r="X38" s="17"/>
-      <c r="Y38" s="17"/>
-      <c r="Z38" s="17"/>
-      <c r="AA38" s="17"/>
-      <c r="AB38" s="17"/>
-      <c r="AC38" s="17"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+      <c r="AC38" s="11"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9"/>
@@ -1605,7 +1853,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="12"/>
-      <c r="K39" s="15"/>
+      <c r="K39" s="13"/>
       <c r="L39" s="11"/>
       <c r="M39" s="11"/>
       <c r="N39" s="11"/>
@@ -1636,7 +1884,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="12"/>
-      <c r="K40" s="15"/>
+      <c r="K40" s="13"/>
       <c r="L40" s="11"/>
       <c r="M40" s="11"/>
       <c r="N40" s="11"/>
@@ -1680,12 +1928,12 @@
       <c r="U41" s="17"/>
       <c r="V41" s="17"/>
       <c r="W41" s="17"/>
-      <c r="X41" s="11"/>
-      <c r="Y41" s="11"/>
-      <c r="Z41" s="11"/>
-      <c r="AA41" s="11"/>
-      <c r="AB41" s="11"/>
-      <c r="AC41" s="11"/>
+      <c r="X41" s="17"/>
+      <c r="Y41" s="17"/>
+      <c r="Z41" s="17"/>
+      <c r="AA41" s="17"/>
+      <c r="AB41" s="17"/>
+      <c r="AC41" s="17"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9"/>
@@ -1705,18 +1953,18 @@
       <c r="O42" s="11"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
-      <c r="U42" s="11"/>
-      <c r="V42" s="11"/>
-      <c r="W42" s="11"/>
-      <c r="X42" s="11"/>
-      <c r="Y42" s="11"/>
-      <c r="Z42" s="11"/>
-      <c r="AA42" s="11"/>
-      <c r="AB42" s="11"/>
-      <c r="AC42" s="11"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
+      <c r="Z42" s="17"/>
+      <c r="AA42" s="17"/>
+      <c r="AB42" s="17"/>
+      <c r="AC42" s="17"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9"/>
@@ -1736,12 +1984,12 @@
       <c r="O43" s="11"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="11"/>
-      <c r="T43" s="11"/>
-      <c r="U43" s="11"/>
-      <c r="V43" s="11"/>
-      <c r="W43" s="11"/>
+      <c r="R43" s="17"/>
+      <c r="S43" s="17"/>
+      <c r="T43" s="17"/>
+      <c r="U43" s="17"/>
+      <c r="V43" s="17"/>
+      <c r="W43" s="17"/>
       <c r="X43" s="11"/>
       <c r="Y43" s="11"/>
       <c r="Z43" s="11"/>
@@ -1767,12 +2015,12 @@
       <c r="O44" s="11"/>
       <c r="P44" s="11"/>
       <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-      <c r="S44" s="11"/>
-      <c r="T44" s="11"/>
-      <c r="U44" s="11"/>
-      <c r="V44" s="11"/>
-      <c r="W44" s="11"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+      <c r="W44" s="17"/>
       <c r="X44" s="11"/>
       <c r="Y44" s="11"/>
       <c r="Z44" s="11"/>
@@ -1798,12 +2046,12 @@
       <c r="O45" s="11"/>
       <c r="P45" s="11"/>
       <c r="Q45" s="11"/>
-      <c r="R45" s="17"/>
-      <c r="S45" s="17"/>
-      <c r="T45" s="17"/>
-      <c r="U45" s="17"/>
-      <c r="V45" s="17"/>
-      <c r="W45" s="17"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
       <c r="X45" s="11"/>
       <c r="Y45" s="11"/>
       <c r="Z45" s="11"/>
@@ -1829,12 +2077,12 @@
       <c r="O46" s="11"/>
       <c r="P46" s="11"/>
       <c r="Q46" s="11"/>
-      <c r="R46" s="17"/>
-      <c r="S46" s="17"/>
-      <c r="T46" s="17"/>
-      <c r="U46" s="17"/>
-      <c r="V46" s="17"/>
-      <c r="W46" s="17"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
       <c r="X46" s="11"/>
       <c r="Y46" s="11"/>
       <c r="Z46" s="11"/>
@@ -1860,18 +2108,18 @@
       <c r="O47" s="11"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="11"/>
-      <c r="R47" s="17"/>
-      <c r="S47" s="17"/>
-      <c r="T47" s="17"/>
-      <c r="U47" s="17"/>
-      <c r="V47" s="17"/>
-      <c r="W47" s="17"/>
-      <c r="X47" s="17"/>
-      <c r="Y47" s="17"/>
-      <c r="Z47" s="17"/>
-      <c r="AA47" s="17"/>
-      <c r="AB47" s="17"/>
-      <c r="AC47" s="17"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+      <c r="Y47" s="11"/>
+      <c r="Z47" s="11"/>
+      <c r="AA47" s="11"/>
+      <c r="AB47" s="11"/>
+      <c r="AC47" s="11"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9"/>
@@ -1891,18 +2139,18 @@
       <c r="O48" s="11"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="11"/>
-      <c r="R48" s="17"/>
-      <c r="S48" s="17"/>
-      <c r="T48" s="17"/>
-      <c r="U48" s="17"/>
-      <c r="V48" s="17"/>
-      <c r="W48" s="17"/>
-      <c r="X48" s="17"/>
-      <c r="Y48" s="17"/>
-      <c r="Z48" s="17"/>
-      <c r="AA48" s="17"/>
-      <c r="AB48" s="17"/>
-      <c r="AC48" s="17"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+      <c r="Y48" s="11"/>
+      <c r="Z48" s="11"/>
+      <c r="AA48" s="11"/>
+      <c r="AB48" s="11"/>
+      <c r="AC48" s="11"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9"/>
@@ -1922,18 +2170,18 @@
       <c r="O49" s="11"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="11"/>
-      <c r="R49" s="17"/>
-      <c r="S49" s="17"/>
-      <c r="T49" s="17"/>
-      <c r="U49" s="17"/>
-      <c r="V49" s="17"/>
-      <c r="W49" s="17"/>
-      <c r="X49" s="17"/>
-      <c r="Y49" s="17"/>
-      <c r="Z49" s="17"/>
-      <c r="AA49" s="17"/>
-      <c r="AB49" s="17"/>
-      <c r="AC49" s="17"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11"/>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+      <c r="Y49" s="11"/>
+      <c r="Z49" s="11"/>
+      <c r="AA49" s="11"/>
+      <c r="AB49" s="11"/>
+      <c r="AC49" s="11"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9"/>
@@ -1953,18 +2201,18 @@
       <c r="O50" s="11"/>
       <c r="P50" s="11"/>
       <c r="Q50" s="11"/>
-      <c r="R50" s="17"/>
-      <c r="S50" s="17"/>
-      <c r="T50" s="17"/>
-      <c r="U50" s="17"/>
-      <c r="V50" s="17"/>
-      <c r="W50" s="17"/>
-      <c r="X50" s="17"/>
-      <c r="Y50" s="17"/>
-      <c r="Z50" s="17"/>
-      <c r="AA50" s="17"/>
-      <c r="AB50" s="17"/>
-      <c r="AC50" s="17"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
+      <c r="Y50" s="11"/>
+      <c r="Z50" s="11"/>
+      <c r="AA50" s="11"/>
+      <c r="AB50" s="11"/>
+      <c r="AC50" s="11"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9"/>
@@ -1977,19 +2225,19 @@
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
       <c r="J51" s="12"/>
-      <c r="K51" s="13"/>
+      <c r="K51" s="15"/>
       <c r="L51" s="11"/>
       <c r="M51" s="11"/>
       <c r="N51" s="11"/>
       <c r="O51" s="11"/>
       <c r="P51" s="11"/>
       <c r="Q51" s="11"/>
-      <c r="R51" s="17"/>
-      <c r="S51" s="17"/>
-      <c r="T51" s="17"/>
-      <c r="U51" s="17"/>
-      <c r="V51" s="17"/>
-      <c r="W51" s="17"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="11"/>
+      <c r="U51" s="11"/>
+      <c r="V51" s="11"/>
+      <c r="W51" s="11"/>
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
       <c r="Z51" s="11"/>
@@ -2008,19 +2256,19 @@
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
       <c r="J52" s="12"/>
-      <c r="K52" s="13"/>
+      <c r="K52" s="15"/>
       <c r="L52" s="11"/>
       <c r="M52" s="11"/>
       <c r="N52" s="11"/>
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
       <c r="Q52" s="11"/>
-      <c r="R52" s="17"/>
-      <c r="S52" s="17"/>
-      <c r="T52" s="17"/>
-      <c r="U52" s="17"/>
-      <c r="V52" s="17"/>
-      <c r="W52" s="17"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="11"/>
+      <c r="T52" s="11"/>
+      <c r="U52" s="11"/>
+      <c r="V52" s="11"/>
+      <c r="W52" s="11"/>
       <c r="X52" s="11"/>
       <c r="Y52" s="11"/>
       <c r="Z52" s="11"/>
@@ -2039,7 +2287,7 @@
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
       <c r="J53" s="12"/>
-      <c r="K53" s="13"/>
+      <c r="K53" s="15"/>
       <c r="L53" s="11"/>
       <c r="M53" s="11"/>
       <c r="N53" s="11"/>
@@ -2070,7 +2318,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
       <c r="J54" s="12"/>
-      <c r="K54" s="13"/>
+      <c r="K54" s="15"/>
       <c r="L54" s="11"/>
       <c r="M54" s="11"/>
       <c r="N54" s="11"/>
@@ -2101,7 +2349,7 @@
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="J55" s="12"/>
-      <c r="K55" s="13"/>
+      <c r="K55" s="15"/>
       <c r="L55" s="11"/>
       <c r="M55" s="11"/>
       <c r="N55" s="11"/>
@@ -2132,7 +2380,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
       <c r="J56" s="12"/>
-      <c r="K56" s="13"/>
+      <c r="K56" s="15"/>
       <c r="L56" s="11"/>
       <c r="M56" s="11"/>
       <c r="N56" s="11"/>
@@ -2163,7 +2411,7 @@
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
       <c r="J57" s="12"/>
-      <c r="K57" s="13"/>
+      <c r="K57" s="15"/>
       <c r="L57" s="11"/>
       <c r="M57" s="11"/>
       <c r="N57" s="11"/>
@@ -2194,7 +2442,7 @@
       <c r="H58" s="11"/>
       <c r="I58" s="11"/>
       <c r="J58" s="12"/>
-      <c r="K58" s="13"/>
+      <c r="K58" s="15"/>
       <c r="L58" s="11"/>
       <c r="M58" s="11"/>
       <c r="N58" s="11"/>
@@ -2349,7 +2597,7 @@
       <c r="H63" s="11"/>
       <c r="I63" s="11"/>
       <c r="J63" s="12"/>
-      <c r="K63" s="15"/>
+      <c r="K63" s="19"/>
       <c r="L63" s="11"/>
       <c r="M63" s="11"/>
       <c r="N63" s="11"/>
@@ -2357,17 +2605,17 @@
       <c r="P63" s="11"/>
       <c r="Q63" s="11"/>
       <c r="R63" s="11"/>
-      <c r="S63" s="11"/>
-      <c r="T63" s="11"/>
+      <c r="S63" s="16"/>
+      <c r="T63" s="16"/>
       <c r="U63" s="11"/>
       <c r="V63" s="11"/>
       <c r="W63" s="11"/>
-      <c r="X63" s="11"/>
-      <c r="Y63" s="11"/>
-      <c r="Z63" s="11"/>
-      <c r="AA63" s="11"/>
-      <c r="AB63" s="11"/>
-      <c r="AC63" s="11"/>
+      <c r="X63" s="16"/>
+      <c r="Y63" s="16"/>
+      <c r="Z63" s="16"/>
+      <c r="AA63" s="16"/>
+      <c r="AB63" s="16"/>
+      <c r="AC63" s="16"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9"/>
@@ -2418,12 +2666,12 @@
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
       <c r="Q65" s="11"/>
-      <c r="R65" s="11"/>
-      <c r="S65" s="11"/>
-      <c r="T65" s="11"/>
-      <c r="U65" s="11"/>
-      <c r="V65" s="11"/>
-      <c r="W65" s="11"/>
+      <c r="R65" s="16"/>
+      <c r="S65" s="16"/>
+      <c r="T65" s="16"/>
+      <c r="U65" s="16"/>
+      <c r="V65" s="16"/>
+      <c r="W65" s="16"/>
       <c r="X65" s="11"/>
       <c r="Y65" s="11"/>
       <c r="Z65" s="11"/>
@@ -2449,12 +2697,12 @@
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
       <c r="Q66" s="11"/>
-      <c r="R66" s="11"/>
-      <c r="S66" s="11"/>
-      <c r="T66" s="11"/>
-      <c r="U66" s="11"/>
-      <c r="V66" s="11"/>
-      <c r="W66" s="11"/>
+      <c r="R66" s="16"/>
+      <c r="S66" s="16"/>
+      <c r="T66" s="16"/>
+      <c r="U66" s="16"/>
+      <c r="V66" s="16"/>
+      <c r="W66" s="16"/>
       <c r="X66" s="11"/>
       <c r="Y66" s="11"/>
       <c r="Z66" s="11"/>
@@ -2480,12 +2728,12 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
       <c r="Q67" s="11"/>
-      <c r="R67" s="11"/>
-      <c r="S67" s="11"/>
-      <c r="T67" s="11"/>
-      <c r="U67" s="11"/>
-      <c r="V67" s="11"/>
-      <c r="W67" s="11"/>
+      <c r="R67" s="16"/>
+      <c r="S67" s="16"/>
+      <c r="T67" s="16"/>
+      <c r="U67" s="16"/>
+      <c r="V67" s="16"/>
+      <c r="W67" s="16"/>
       <c r="X67" s="11"/>
       <c r="Y67" s="11"/>
       <c r="Z67" s="11"/>
@@ -2542,12 +2790,12 @@
       <c r="O69" s="11"/>
       <c r="P69" s="11"/>
       <c r="Q69" s="11"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="11"/>
-      <c r="T69" s="11"/>
-      <c r="U69" s="11"/>
-      <c r="V69" s="11"/>
-      <c r="W69" s="11"/>
+      <c r="R69" s="16"/>
+      <c r="S69" s="16"/>
+      <c r="T69" s="16"/>
+      <c r="U69" s="16"/>
+      <c r="V69" s="16"/>
+      <c r="W69" s="16"/>
       <c r="X69" s="11"/>
       <c r="Y69" s="11"/>
       <c r="Z69" s="11"/>
@@ -2573,12 +2821,12 @@
       <c r="O70" s="11"/>
       <c r="P70" s="11"/>
       <c r="Q70" s="11"/>
-      <c r="R70" s="11"/>
-      <c r="S70" s="11"/>
-      <c r="T70" s="11"/>
-      <c r="U70" s="11"/>
-      <c r="V70" s="11"/>
-      <c r="W70" s="11"/>
+      <c r="R70" s="16"/>
+      <c r="S70" s="16"/>
+      <c r="T70" s="16"/>
+      <c r="U70" s="16"/>
+      <c r="V70" s="16"/>
+      <c r="W70" s="16"/>
       <c r="X70" s="11"/>
       <c r="Y70" s="11"/>
       <c r="Z70" s="11"/>
@@ -2597,25 +2845,25 @@
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
       <c r="J71" s="12"/>
-      <c r="K71" s="19"/>
+      <c r="K71" s="15"/>
       <c r="L71" s="11"/>
       <c r="M71" s="11"/>
       <c r="N71" s="11"/>
       <c r="O71" s="11"/>
       <c r="P71" s="11"/>
       <c r="Q71" s="11"/>
-      <c r="R71" s="11"/>
+      <c r="R71" s="16"/>
       <c r="S71" s="16"/>
       <c r="T71" s="16"/>
-      <c r="U71" s="11"/>
-      <c r="V71" s="11"/>
-      <c r="W71" s="11"/>
-      <c r="X71" s="16"/>
-      <c r="Y71" s="16"/>
-      <c r="Z71" s="16"/>
-      <c r="AA71" s="16"/>
-      <c r="AB71" s="16"/>
-      <c r="AC71" s="16"/>
+      <c r="U71" s="16"/>
+      <c r="V71" s="16"/>
+      <c r="W71" s="16"/>
+      <c r="X71" s="11"/>
+      <c r="Y71" s="11"/>
+      <c r="Z71" s="11"/>
+      <c r="AA71" s="11"/>
+      <c r="AB71" s="11"/>
+      <c r="AC71" s="11"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9"/>
@@ -2628,7 +2876,7 @@
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
       <c r="J72" s="12"/>
-      <c r="K72" s="15"/>
+      <c r="K72" s="13"/>
       <c r="L72" s="11"/>
       <c r="M72" s="11"/>
       <c r="N72" s="11"/>
@@ -2638,270 +2886,22 @@
       <c r="R72" s="11"/>
       <c r="S72" s="11"/>
       <c r="T72" s="11"/>
-      <c r="U72" s="11"/>
-      <c r="V72" s="11"/>
-      <c r="W72" s="11"/>
+      <c r="U72" s="17"/>
+      <c r="V72" s="17"/>
+      <c r="W72" s="17"/>
       <c r="X72" s="11"/>
       <c r="Y72" s="11"/>
       <c r="Z72" s="11"/>
-      <c r="AA72" s="11"/>
-      <c r="AB72" s="11"/>
-      <c r="AC72" s="11"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="9"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="12"/>
-      <c r="K73" s="15"/>
-      <c r="L73" s="11"/>
-      <c r="M73" s="11"/>
-      <c r="N73" s="11"/>
-      <c r="O73" s="11"/>
-      <c r="P73" s="11"/>
-      <c r="Q73" s="11"/>
-      <c r="R73" s="16"/>
-      <c r="S73" s="16"/>
-      <c r="T73" s="16"/>
-      <c r="U73" s="16"/>
-      <c r="V73" s="16"/>
-      <c r="W73" s="16"/>
-      <c r="X73" s="11"/>
-      <c r="Y73" s="11"/>
-      <c r="Z73" s="11"/>
-      <c r="AA73" s="11"/>
-      <c r="AB73" s="11"/>
-      <c r="AC73" s="11"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="9"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="12"/>
-      <c r="K74" s="15"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
-      <c r="O74" s="11"/>
-      <c r="P74" s="11"/>
-      <c r="Q74" s="11"/>
-      <c r="R74" s="16"/>
-      <c r="S74" s="16"/>
-      <c r="T74" s="16"/>
-      <c r="U74" s="16"/>
-      <c r="V74" s="16"/>
-      <c r="W74" s="16"/>
-      <c r="X74" s="11"/>
-      <c r="Y74" s="11"/>
-      <c r="Z74" s="11"/>
-      <c r="AA74" s="11"/>
-      <c r="AB74" s="11"/>
-      <c r="AC74" s="11"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="9"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="12"/>
-      <c r="K75" s="15"/>
-      <c r="L75" s="11"/>
-      <c r="M75" s="11"/>
-      <c r="N75" s="11"/>
-      <c r="O75" s="11"/>
-      <c r="P75" s="11"/>
-      <c r="Q75" s="11"/>
-      <c r="R75" s="16"/>
-      <c r="S75" s="16"/>
-      <c r="T75" s="16"/>
-      <c r="U75" s="16"/>
-      <c r="V75" s="16"/>
-      <c r="W75" s="16"/>
-      <c r="X75" s="11"/>
-      <c r="Y75" s="11"/>
-      <c r="Z75" s="11"/>
-      <c r="AA75" s="11"/>
-      <c r="AB75" s="11"/>
-      <c r="AC75" s="11"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="9"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="12"/>
-      <c r="K76" s="15"/>
-      <c r="L76" s="11"/>
-      <c r="M76" s="11"/>
-      <c r="N76" s="11"/>
-      <c r="O76" s="11"/>
-      <c r="P76" s="11"/>
-      <c r="Q76" s="11"/>
-      <c r="R76" s="11"/>
-      <c r="S76" s="11"/>
-      <c r="T76" s="11"/>
-      <c r="U76" s="11"/>
-      <c r="V76" s="11"/>
-      <c r="W76" s="11"/>
-      <c r="X76" s="11"/>
-      <c r="Y76" s="11"/>
-      <c r="Z76" s="11"/>
-      <c r="AA76" s="11"/>
-      <c r="AB76" s="11"/>
-      <c r="AC76" s="11"/>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="9"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="12"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="11"/>
-      <c r="M77" s="11"/>
-      <c r="N77" s="11"/>
-      <c r="O77" s="11"/>
-      <c r="P77" s="11"/>
-      <c r="Q77" s="11"/>
-      <c r="R77" s="16"/>
-      <c r="S77" s="16"/>
-      <c r="T77" s="16"/>
-      <c r="U77" s="16"/>
-      <c r="V77" s="16"/>
-      <c r="W77" s="16"/>
-      <c r="X77" s="11"/>
-      <c r="Y77" s="11"/>
-      <c r="Z77" s="11"/>
-      <c r="AA77" s="11"/>
-      <c r="AB77" s="11"/>
-      <c r="AC77" s="11"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="12"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="11"/>
-      <c r="M78" s="11"/>
-      <c r="N78" s="11"/>
-      <c r="O78" s="11"/>
-      <c r="P78" s="11"/>
-      <c r="Q78" s="11"/>
-      <c r="R78" s="16"/>
-      <c r="S78" s="16"/>
-      <c r="T78" s="16"/>
-      <c r="U78" s="16"/>
-      <c r="V78" s="16"/>
-      <c r="W78" s="16"/>
-      <c r="X78" s="11"/>
-      <c r="Y78" s="11"/>
-      <c r="Z78" s="11"/>
-      <c r="AA78" s="11"/>
-      <c r="AB78" s="11"/>
-      <c r="AC78" s="11"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="9"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="12"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="11"/>
-      <c r="M79" s="11"/>
-      <c r="N79" s="11"/>
-      <c r="O79" s="11"/>
-      <c r="P79" s="11"/>
-      <c r="Q79" s="11"/>
-      <c r="R79" s="16"/>
-      <c r="S79" s="16"/>
-      <c r="T79" s="16"/>
-      <c r="U79" s="16"/>
-      <c r="V79" s="16"/>
-      <c r="W79" s="16"/>
-      <c r="X79" s="11"/>
-      <c r="Y79" s="11"/>
-      <c r="Z79" s="11"/>
-      <c r="AA79" s="11"/>
-      <c r="AB79" s="11"/>
-      <c r="AC79" s="11"/>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="9"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="12"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="11"/>
-      <c r="M80" s="11"/>
-      <c r="N80" s="11"/>
-      <c r="O80" s="11"/>
-      <c r="P80" s="11"/>
-      <c r="Q80" s="11"/>
-      <c r="R80" s="11"/>
-      <c r="S80" s="11"/>
-      <c r="T80" s="11"/>
-      <c r="U80" s="17"/>
-      <c r="V80" s="17"/>
-      <c r="W80" s="17"/>
-      <c r="X80" s="11"/>
-      <c r="Y80" s="11"/>
-      <c r="Z80" s="11"/>
-      <c r="AA80" s="17"/>
-      <c r="AB80" s="17"/>
-      <c r="AC80" s="17"/>
+      <c r="AA72" s="17"/>
+      <c r="AB72" s="17"/>
+      <c r="AC72" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="L9:Q9"/>
-    <mergeCell ref="R9:W9"/>
-    <mergeCell ref="X9:AC9"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="X1:AC1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated template column name
</commit_message>
<xml_diff>
--- a/assets/templates/import-rights-template.xlsx
+++ b/assets/templates/import-rights-template.xlsx
@@ -46,7 +46,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Date
+      <t xml:space="preserve">ContractId Or Date
 </t>
     </r>
     <r>
@@ -58,7 +58,8 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">// specify date if right is created after first statement
+      <t xml:space="preserve">//  Empty by default but 
+specify contractId or date if right is created after first statement
 </t>
     </r>
   </si>
@@ -577,10 +578,10 @@
   <dimension ref="A1:AH72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>

</xml_diff>

<commit_message>
added orgId check on vertical group childrens
</commit_message>
<xml_diff>
--- a/assets/templates/import-rights-template.xlsx
+++ b/assets/templates/import-rights-template.xlsx
@@ -84,8 +84,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">// Org Name
-// Will define BlameId if group</t>
+      <t xml:space="preserve">// Org Name</t>
     </r>
   </si>
   <si>
@@ -620,11 +619,11 @@
   </sheetPr>
   <dimension ref="A1:AE72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA3" activeCellId="0" sqref="A3:AA72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.85"/>

</xml_diff>

<commit_message>
#9501 & part of #9493
</commit_message>
<xml_diff>
--- a/assets/templates/import-rights-template.xlsx
+++ b/assets/templates/import-rights-template.xlsx
@@ -162,31 +162,7 @@
     <t xml:space="preserve">Target Percentage</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Contract ID Or Date
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="6"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">//  Empty by default but 
-specify contractId or date if right is created after first statement
-</t>
-    </r>
+    <t xml:space="preserve">Contract ID</t>
   </si>
 </sst>
 </file>
@@ -619,11 +595,11 @@
   </sheetPr>
   <dimension ref="A1:AE72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA3" activeCellId="0" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.85"/>

</xml_diff>